<commit_message>
Updated documents and values
</commit_message>
<xml_diff>
--- a/AcademicStages.xlsx
+++ b/AcademicStages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/as822/Documents/GitHub/FLXSUS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1D02E4-2266-2C4B-863D-C7B411D2A259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E89307-CEED-5849-90EA-DDBD7882D863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="63200" yWindow="-5480" windowWidth="34400" windowHeight="28300" activeTab="2" xr2:uid="{192DB08B-ABE8-C24A-96C6-4E8A2DD06EAD}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$511</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6162,67 +6162,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -33623,7 +33563,7 @@
     <sortCondition ref="A2:A141"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33633,9 +33573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A138E2A-342A-ED42-8FB2-9526932A44B0}">
   <dimension ref="A1:W116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G68" workbookViewId="0">
-      <selection activeCell="U96" sqref="U96"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -38684,79 +38622,49 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V1:V104 V127:V1048576 V106:V116">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Other">
+  <conditionalFormatting sqref="V1:V104 V106:V116 V127:V1048576">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",V1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Other">
+  <conditionalFormatting sqref="W2:W5">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W4">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W5">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W7">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Other">
+  <conditionalFormatting sqref="W7:W9">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W8">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W9">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W39">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Other">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43:W44">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Other">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Other">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W48">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Other">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W53">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Other">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W53)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W77">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Other">
+  <conditionalFormatting sqref="W77:W78">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Other">
       <formula>NOT(ISERROR(SEARCH("Other",W77)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W78">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Other">
-      <formula>NOT(ISERROR(SEARCH("Other",W78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>